<commit_message>
update parameter mapping file #1
</commit_message>
<xml_diff>
--- a/inst/extdata/ExampleCont.xlsx
+++ b/inst/extdata/ExampleCont.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\AquaSensR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7859D2-F241-438B-8D8D-E6CCE70E0831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4053188B-4296-4A05-90F0-D0A9FDC27AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F8A2AE6C-EDC3-4226-B9D4-2DE8A25DC7E8}"/>
+    <workbookView xWindow="32460" yWindow="825" windowWidth="18270" windowHeight="14325" xr2:uid="{F8A2AE6C-EDC3-4226-B9D4-2DE8A25DC7E8}"/>
   </bookViews>
   <sheets>
     <sheet name="YSI_SUD-DO_LoggerRaw" sheetId="1" r:id="rId1"/>
@@ -40,19 +40,19 @@
     <t>DO_pctsat</t>
   </si>
   <si>
-    <t>DO_mg_L</t>
-  </si>
-  <si>
     <t>Conductivity_uS_cm</t>
-  </si>
-  <si>
-    <t>Salinity_psu</t>
   </si>
   <si>
     <t>pH_SU</t>
   </si>
   <si>
-    <t>TDS_mg_L</t>
+    <t>DO_mg_l</t>
+  </si>
+  <si>
+    <t>TDS_mg_l</t>
+  </si>
+  <si>
+    <t>Salinity_ppt</t>
   </si>
 </sst>
 </file>
@@ -918,7 +918,7 @@
   <dimension ref="A1:J928"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -952,19 +952,19 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>